<commit_message>
Add gropuing of virus strains
</commit_message>
<xml_diff>
--- a/pneumoviridae/family.xlsx
+++ b/pneumoviridae/family.xlsx
@@ -17,7 +17,7 @@
     <author>tc={5CCD2509-F247-436F-9840-D50D29C9A459}</author>
   </authors>
   <commentList>
-    <comment ref="F8" authorId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -37,7 +37,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="1">
+    <comment ref="H12" authorId="1">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>virus_id</t>
   </si>
@@ -69,6 +69,12 @@
     <t>virus_name</t>
   </si>
   <si>
+    <t>goup_abbreviation</t>
+  </si>
+  <si>
+    <t>group_virus_name</t>
+  </si>
+  <si>
     <t>genus_name</t>
   </si>
   <si>
@@ -153,6 +159,9 @@
     <t>Human metapneumovirus A1</t>
   </si>
   <si>
+    <t>hMPV</t>
+  </si>
+  <si>
     <t>Human metapneumovirus</t>
   </si>
   <si>
@@ -193,6 +202,12 @@
   </si>
   <si>
     <t>Human respiratory syncytial virus A2</t>
+  </si>
+  <si>
+    <t>hRSV</t>
+  </si>
+  <si>
+    <t>Human respiratory syncytial virus</t>
   </si>
   <si>
     <t>'HRSV B1 AF013254'</t>
@@ -211,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -221,11 +236,6 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="15"/>
@@ -238,12 +248,18 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -256,16 +272,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -279,13 +295,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -305,6 +321,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -326,10 +343,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -506,11 +523,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -519,33 +539,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -784,12 +804,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1070,7 +1090,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1338,7 +1358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1346,17 +1366,18 @@
   <cols>
     <col min="1" max="1" width="24.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.8516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.3516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1719" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1719" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3359" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.8516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.1719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.3516" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.1719" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.1719" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1">
@@ -1396,326 +1417,380 @@
       <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
+      <c r="M1" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>15</v>
-      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>18</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>15</v>
-      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>18</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>15</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>18</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>15</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>18</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>15</v>
-      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>18</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>18</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>17</v>
+      </c>
       <c r="H8" t="s" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="J8" t="s" s="2">
+        <v>35</v>
+      </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="E9" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="2">
+      <c r="F9" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" t="s" s="2">
         <v>35</v>
       </c>
-      <c r="D9" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>17</v>
+      </c>
       <c r="H10" t="s" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" t="s" s="2">
+        <v>35</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="G11" t="s" s="2">
+        <v>17</v>
+      </c>
       <c r="H11" t="s" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" t="s" s="2">
+        <v>35</v>
+      </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>35</v>
+      </c>
       <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="J13" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s" s="2">
+        <v>35</v>
+      </c>
       <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>